<commit_message>
added depth into the recursion
</commit_message>
<xml_diff>
--- a/test_recursed.xlsx
+++ b/test_recursed.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="60" yWindow="1946" windowWidth="16200" windowHeight="9951" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,7 +25,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +47,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +72,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,13 +435,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -439,39 +449,20 @@
           <t>Ошибки\Коды</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" t="inlineStr">
         <is>
           <t>Код (4,2)</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Код (5,2)</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Код (6,2)</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Код (7,2)</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Код (8,2)</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Код (9,2)</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Код (10,2)</t>
         </is>
       </c>
     </row>
@@ -481,9 +472,6 @@
           <t>max</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>100</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -491,26 +479,14 @@
           <t>max+1</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
@@ -519,14 +495,14 @@
           <t>max+2</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="5">
@@ -535,14 +511,14 @@
           <t>max+3</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -551,14 +527,14 @@
           <t>max+4</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -567,14 +543,14 @@
           <t>max+5</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -586,8 +562,8 @@
       <c r="C8" t="n">
         <v>0</v>
       </c>
-      <c r="D8" t="n">
-        <v>3</v>
+      <c r="E8" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -597,10 +573,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -609,8 +585,11 @@
           <t>max+8</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>1</v>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -619,7 +598,7 @@
           <t>max+9</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -629,7 +608,7 @@
           <t>max+10</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change testing and add tuninig calculations
</commit_message>
<xml_diff>
--- a/test_recursed.xlsx
+++ b/test_recursed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="60" yWindow="1946" windowWidth="16200" windowHeight="9951" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -435,20 +435,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ошибки\Коды</t>
-        </is>
-      </c>
+      <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="n"/>
       <c r="C1" t="inlineStr">
         <is>
@@ -469,124 +465,109 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>max</t>
-        </is>
+          <t>max+1</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>31</v>
+      </c>
+      <c r="E2" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>max+1</t>
+          <t>max+2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>max+2</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
+          <t>max+3</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>max+3</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+          <t>max+4</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
       <c r="E5" t="n">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>max+4</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
+          <t>max+5</t>
+        </is>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>max+5</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
+          <t>max+6</t>
+        </is>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>max+6</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
+          <t>max+7</t>
+        </is>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>max+7</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>7</v>
+          <t>max+8</t>
+        </is>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>max+8</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>100</v>
+          <t>max+9</t>
+        </is>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -595,20 +576,10 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>max+9</t>
+          <t>max+10</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>max+10</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>